<commit_message>
config(EJ2-24078): moved the samples to ej2-aspcore github repository
</commit_message>
<xml_diff>
--- a/wwwroot/XlsIO/CFTemplate.xlsx
+++ b/wwwroot/XlsIO/CFTemplate.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Syncfusion\Windows\16.4.0.52\Common\Data\XlsIO\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C4D263-411F-402C-8F4E-531AB32DC5B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="8415" windowHeight="4050"/>
+    <workbookView xWindow="120" yWindow="80" windowWidth="8420" windowHeight="4050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr fullPrecision="1" calcId="125725"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>SalesPerson</t>
   </si>
@@ -156,37 +162,34 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <color theme="1"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <color theme="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <color theme="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="64"/>
-        <bgColor indexed="65"/>
-      </patternFill>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor indexed="64"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="5">
@@ -253,28 +256,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs>
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -562,23 +574,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:E46"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="AE84" sqref="AE84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="23.99609375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="32.8515625" customWidth="1"/>
-    <col min="4" max="4" width="42.99609375" customWidth="1"/>
-    <col min="5" max="5" width="16.99609375" customWidth="1"/>
+    <col min="1" max="1" width="2.453125" customWidth="1"/>
+    <col min="2" max="2" width="24" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" customWidth="1"/>
+    <col min="4" max="4" width="19.26953125" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" ht="18.75">
+    <row r="3" spans="2:5" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B3" s="7" t="s">
         <v>8</v>
       </c>
@@ -586,13 +598,13 @@
       <c r="D3" s="8"/>
       <c r="E3" s="9"/>
     </row>
-    <row r="4" spans="2:5" ht="15">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B4" s="6"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="2:5" ht="15">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
@@ -606,13 +618,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="15">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B6" s="6"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="2:5" ht="15">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B7" s="6" t="s">
         <v>3</v>
       </c>
@@ -620,13 +632,13 @@
         <v>45000</v>
       </c>
       <c r="D7" s="3">
-        <v>58000</v>
+        <v>60000</v>
       </c>
       <c r="E7" s="4">
-        <v>0.29</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="15">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B8" s="6" t="s">
         <v>4</v>
       </c>
@@ -640,7 +652,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="15">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B9" s="6" t="s">
         <v>5</v>
       </c>
@@ -654,7 +666,7 @@
         <v>-0.15</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="15">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B10" s="6" t="s">
         <v>6</v>
       </c>
@@ -662,13 +674,13 @@
         <v>56500</v>
       </c>
       <c r="D10" s="3">
-        <v>33600</v>
+        <v>32000</v>
       </c>
       <c r="E10" s="4">
         <v>-0.4</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="15">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B11" s="6" t="s">
         <v>7</v>
       </c>
@@ -682,7 +694,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="15">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B12" s="6" t="s">
         <v>9</v>
       </c>
@@ -693,10 +705,10 @@
         <v>58000</v>
       </c>
       <c r="E12" s="4">
-        <v>0.29</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" ht="15">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B13" s="6" t="s">
         <v>43</v>
       </c>
@@ -710,7 +722,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="14" spans="2:5" ht="15">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B14" s="6" t="s">
         <v>10</v>
       </c>
@@ -724,7 +736,7 @@
         <v>-0.15</v>
       </c>
     </row>
-    <row r="15" spans="2:5" ht="15">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B15" s="6" t="s">
         <v>11</v>
       </c>
@@ -738,7 +750,7 @@
         <v>-0.4</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="15">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B16" s="6" t="s">
         <v>12</v>
       </c>
@@ -752,7 +764,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="15">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" s="6" t="s">
         <v>13</v>
       </c>
@@ -760,13 +772,13 @@
         <v>45000</v>
       </c>
       <c r="D17" s="3">
-        <v>58000</v>
+        <v>58500</v>
       </c>
       <c r="E17" s="4">
-        <v>0.29</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="15">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B18" s="6" t="s">
         <v>14</v>
       </c>
@@ -780,7 +792,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="15">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" s="6" t="s">
         <v>15</v>
       </c>
@@ -794,7 +806,7 @@
         <v>-0.15</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="15">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" s="6" t="s">
         <v>16</v>
       </c>
@@ -808,7 +820,7 @@
         <v>-0.4</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="15">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B21" s="6" t="s">
         <v>17</v>
       </c>
@@ -822,7 +834,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="22" spans="2:5" ht="15">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B22" s="6" t="s">
         <v>18</v>
       </c>
@@ -833,10 +845,10 @@
         <v>58000</v>
       </c>
       <c r="E22" s="4">
-        <v>0.29</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" ht="15">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B23" s="6" t="s">
         <v>19</v>
       </c>
@@ -844,13 +856,13 @@
         <v>34000</v>
       </c>
       <c r="D23" s="3">
-        <v>65000</v>
+        <v>65700</v>
       </c>
       <c r="E23" s="4">
         <v>0.91</v>
       </c>
     </row>
-    <row r="24" spans="2:5" ht="15">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B24" s="6" t="s">
         <v>20</v>
       </c>
@@ -864,7 +876,7 @@
         <v>-0.15</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="15">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B25" s="6" t="s">
         <v>21</v>
       </c>
@@ -878,7 +890,7 @@
         <v>-0.4</v>
       </c>
     </row>
-    <row r="26" spans="2:5" ht="15">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B26" s="6" t="s">
         <v>22</v>
       </c>
@@ -892,7 +904,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="27" spans="2:5" ht="15">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B27" s="6" t="s">
         <v>23</v>
       </c>
@@ -903,10 +915,10 @@
         <v>58000</v>
       </c>
       <c r="E27" s="4">
-        <v>0.29</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" ht="15">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B28" s="6" t="s">
         <v>24</v>
       </c>
@@ -920,7 +932,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="29" spans="2:5" ht="15">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B29" s="6" t="s">
         <v>25</v>
       </c>
@@ -934,7 +946,7 @@
         <v>-0.15</v>
       </c>
     </row>
-    <row r="30" spans="2:5" ht="15">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B30" s="6" t="s">
         <v>26</v>
       </c>
@@ -948,7 +960,7 @@
         <v>-0.4</v>
       </c>
     </row>
-    <row r="31" spans="2:5" ht="15">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B31" s="6" t="s">
         <v>27</v>
       </c>
@@ -962,7 +974,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="32" spans="2:5" ht="15">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B32" s="6" t="s">
         <v>28</v>
       </c>
@@ -973,10 +985,10 @@
         <v>58000</v>
       </c>
       <c r="E32" s="4">
-        <v>0.29</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" ht="15">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B33" s="6" t="s">
         <v>29</v>
       </c>
@@ -990,7 +1002,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="34" spans="2:5" ht="15">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B34" s="6" t="s">
         <v>30</v>
       </c>
@@ -1004,7 +1016,7 @@
         <v>-0.15</v>
       </c>
     </row>
-    <row r="35" spans="2:5" ht="15">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B35" s="6" t="s">
         <v>31</v>
       </c>
@@ -1018,7 +1030,7 @@
         <v>-0.4</v>
       </c>
     </row>
-    <row r="36" spans="2:5" ht="15">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B36" s="6" t="s">
         <v>32</v>
       </c>
@@ -1026,13 +1038,13 @@
         <v>46500</v>
       </c>
       <c r="D36" s="3">
-        <v>52000</v>
+        <v>51500</v>
       </c>
       <c r="E36" s="4">
         <v>0.12</v>
       </c>
     </row>
-    <row r="37" spans="2:5" ht="15">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B37" s="6" t="s">
         <v>33</v>
       </c>
@@ -1043,10 +1055,10 @@
         <v>58000</v>
       </c>
       <c r="E37" s="4">
-        <v>0.29</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" ht="15">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B38" s="6" t="s">
         <v>34</v>
       </c>
@@ -1060,7 +1072,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="39" spans="2:5" ht="15">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B39" s="6" t="s">
         <v>35</v>
       </c>
@@ -1074,7 +1086,7 @@
         <v>-0.15</v>
       </c>
     </row>
-    <row r="40" spans="2:5" ht="15">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B40" s="6" t="s">
         <v>36</v>
       </c>
@@ -1088,7 +1100,7 @@
         <v>-0.4</v>
       </c>
     </row>
-    <row r="41" spans="2:5" ht="15">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B41" s="6" t="s">
         <v>37</v>
       </c>
@@ -1102,7 +1114,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="42" spans="2:5" ht="15">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B42" s="6" t="s">
         <v>38</v>
       </c>
@@ -1110,13 +1122,13 @@
         <v>45000</v>
       </c>
       <c r="D42" s="3">
-        <v>58000</v>
+        <v>58300</v>
       </c>
       <c r="E42" s="4">
-        <v>0.29</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" ht="15">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B43" s="6" t="s">
         <v>39</v>
       </c>
@@ -1124,13 +1136,13 @@
         <v>34000</v>
       </c>
       <c r="D43" s="3">
-        <v>65000</v>
+        <v>62400</v>
       </c>
       <c r="E43" s="4">
         <v>0.91</v>
       </c>
     </row>
-    <row r="44" spans="2:5" ht="15">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B44" s="6" t="s">
         <v>42</v>
       </c>
@@ -1144,7 +1156,7 @@
         <v>-0.15</v>
       </c>
     </row>
-    <row r="45" spans="2:5" ht="15">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B45" s="6" t="s">
         <v>40</v>
       </c>
@@ -1158,7 +1170,7 @@
         <v>-0.4</v>
       </c>
     </row>
-    <row r="46" spans="2:5" ht="15">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B46" s="6" t="s">
         <v>41</v>
       </c>
@@ -1177,36 +1189,32 @@
     <mergeCell ref="B3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup pageOrder="downThenOver" orientation="portrait" verticalDpi="0"/>
+  <pageSetup orientation="portrait" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" pageOrder="downThenOver" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" pageOrder="downThenOver" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
sample(EJ2-31339): Release Branch Update
</commit_message>
<xml_diff>
--- a/wwwroot/XlsIO/CFTemplate.xlsx
+++ b/wwwroot/XlsIO/CFTemplate.xlsx
@@ -1,28 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Syncfusion\Windows\16.4.0.52\Common\Data\XlsIO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Syncfusion\Gitlab\WPF\Common\Data\XlsIO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C4D263-411F-402C-8F4E-531AB32DC5B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABF72C9-5593-47B7-A5AD-BA323422751A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="80" windowWidth="8420" windowHeight="4050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="AdvancedCF" sheetId="1" r:id="rId1"/>
+    <sheet name="Top-Bottom Rules" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
   <si>
     <t>SalesPerson</t>
   </si>
@@ -157,17 +164,168 @@
   </si>
   <si>
     <t>Sales Jan- June</t>
+  </si>
+  <si>
+    <t>Students Marks Report</t>
+  </si>
+  <si>
+    <t>Highlighted by Top 10 / Below Average</t>
+  </si>
+  <si>
+    <t>Students</t>
+  </si>
+  <si>
+    <t>Subject 1</t>
+  </si>
+  <si>
+    <t>Subject 2</t>
+  </si>
+  <si>
+    <t>Subject 3</t>
+  </si>
+  <si>
+    <t>Subject 4</t>
+  </si>
+  <si>
+    <t>Subject 5</t>
+  </si>
+  <si>
+    <t>Subject 6</t>
+  </si>
+  <si>
+    <t>Subject 7</t>
+  </si>
+  <si>
+    <t>Subject 8</t>
+  </si>
+  <si>
+    <t>Subject 9</t>
+  </si>
+  <si>
+    <t>Subject 10</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>Student 1</t>
+  </si>
+  <si>
+    <t>Student 2</t>
+  </si>
+  <si>
+    <t>Student 3</t>
+  </si>
+  <si>
+    <t>Student 4</t>
+  </si>
+  <si>
+    <t>Student 5</t>
+  </si>
+  <si>
+    <t>Student 6</t>
+  </si>
+  <si>
+    <t>Student 7</t>
+  </si>
+  <si>
+    <t>Student 8</t>
+  </si>
+  <si>
+    <t>Student 9</t>
+  </si>
+  <si>
+    <t>Student 10</t>
+  </si>
+  <si>
+    <t>Student 11</t>
+  </si>
+  <si>
+    <t>Student 12</t>
+  </si>
+  <si>
+    <t>Student 13</t>
+  </si>
+  <si>
+    <t>Student 14</t>
+  </si>
+  <si>
+    <t>Student 15</t>
+  </si>
+  <si>
+    <t>Student 16</t>
+  </si>
+  <si>
+    <t>Student 17</t>
+  </si>
+  <si>
+    <t>Student 18</t>
+  </si>
+  <si>
+    <t>Student 19</t>
+  </si>
+  <si>
+    <t>Student 20</t>
+  </si>
+  <si>
+    <t>Student 21</t>
+  </si>
+  <si>
+    <t>Student 22</t>
+  </si>
+  <si>
+    <t>Student 23</t>
+  </si>
+  <si>
+    <t>Student 24</t>
+  </si>
+  <si>
+    <t>Student 25</t>
+  </si>
+  <si>
+    <t>Student 26</t>
+  </si>
+  <si>
+    <t>Student 27</t>
+  </si>
+  <si>
+    <t>Student 28</t>
+  </si>
+  <si>
+    <t>Student 29</t>
+  </si>
+  <si>
+    <t>Student 30</t>
+  </si>
+  <si>
+    <t>Below Average</t>
+  </si>
+  <si>
+    <t>Top 10 Rank</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -183,13 +341,77 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFA63B26"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF339966"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -253,32 +475,64 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{FB267ED8-7F92-4CBB-9152-421BB4997FAB}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF339966"/>
+      <color rgb="FF95C45C"/>
+      <color rgb="FFA63B26"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -591,12 +845,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="9"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="19"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B4" s="6"/>
@@ -1194,27 +1448,1534 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE829DD8-420D-4853-A854-F00ADCC9C9DD}">
+  <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="P38" sqref="P38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17.81640625" style="8" customWidth="1"/>
+    <col min="2" max="11" width="10.54296875" style="8" customWidth="1"/>
+    <col min="12" max="12" width="8.453125" style="8" customWidth="1"/>
+    <col min="13" max="13" width="9.81640625" style="8" customWidth="1"/>
+    <col min="14" max="16384" width="8.7265625" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="N1" s="22" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="22"/>
+    </row>
+    <row r="3" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="22"/>
+    </row>
+    <row r="4" spans="1:14" ht="2.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="N5" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="14">
+        <v>99</v>
+      </c>
+      <c r="C6" s="14">
+        <v>97</v>
+      </c>
+      <c r="D6" s="14">
+        <v>93</v>
+      </c>
+      <c r="E6" s="14">
+        <v>100</v>
+      </c>
+      <c r="F6" s="14">
+        <v>91</v>
+      </c>
+      <c r="G6" s="14">
+        <v>92</v>
+      </c>
+      <c r="H6" s="14">
+        <v>92</v>
+      </c>
+      <c r="I6" s="14">
+        <v>95</v>
+      </c>
+      <c r="J6" s="14">
+        <v>91</v>
+      </c>
+      <c r="K6" s="14">
+        <v>89</v>
+      </c>
+      <c r="L6" s="14">
+        <f>SUM(B6:K6)</f>
+        <v>939</v>
+      </c>
+      <c r="M6" s="14">
+        <f>AVERAGE(B6:K6)</f>
+        <v>93.9</v>
+      </c>
+      <c r="N6" s="8">
+        <f>RANK(L6,L6:L35)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="14">
+        <v>86</v>
+      </c>
+      <c r="C7" s="14">
+        <v>88</v>
+      </c>
+      <c r="D7" s="14">
+        <v>90</v>
+      </c>
+      <c r="E7" s="14">
+        <v>92</v>
+      </c>
+      <c r="F7" s="14">
+        <v>91</v>
+      </c>
+      <c r="G7" s="14">
+        <v>87</v>
+      </c>
+      <c r="H7" s="14">
+        <v>96</v>
+      </c>
+      <c r="I7" s="14">
+        <v>75</v>
+      </c>
+      <c r="J7" s="14">
+        <v>80</v>
+      </c>
+      <c r="K7" s="14">
+        <v>92</v>
+      </c>
+      <c r="L7" s="14">
+        <f t="shared" ref="L7:L35" si="0">SUM(B7:K7)</f>
+        <v>877</v>
+      </c>
+      <c r="M7" s="14">
+        <f t="shared" ref="M7:M35" si="1">AVERAGE(B7:K7)</f>
+        <v>87.7</v>
+      </c>
+      <c r="N7" s="8">
+        <f>RANK(L7,L6:L35)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="14">
+        <v>91</v>
+      </c>
+      <c r="C8" s="14">
+        <v>92</v>
+      </c>
+      <c r="D8" s="14">
+        <v>97</v>
+      </c>
+      <c r="E8" s="14">
+        <v>94</v>
+      </c>
+      <c r="F8" s="14">
+        <v>91</v>
+      </c>
+      <c r="G8" s="14">
+        <v>92</v>
+      </c>
+      <c r="H8" s="14">
+        <v>95</v>
+      </c>
+      <c r="I8" s="14">
+        <v>99</v>
+      </c>
+      <c r="J8" s="14">
+        <v>100</v>
+      </c>
+      <c r="K8" s="14">
+        <v>94</v>
+      </c>
+      <c r="L8" s="14">
+        <f t="shared" si="0"/>
+        <v>945</v>
+      </c>
+      <c r="M8" s="14">
+        <f t="shared" si="1"/>
+        <v>94.5</v>
+      </c>
+      <c r="N8" s="8">
+        <f>RANK(L8,L6:L35)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="14">
+        <v>64</v>
+      </c>
+      <c r="C9" s="14">
+        <v>71</v>
+      </c>
+      <c r="D9" s="14">
+        <v>82</v>
+      </c>
+      <c r="E9" s="14">
+        <v>80</v>
+      </c>
+      <c r="F9" s="14">
+        <v>63</v>
+      </c>
+      <c r="G9" s="14">
+        <v>71</v>
+      </c>
+      <c r="H9" s="14">
+        <v>88</v>
+      </c>
+      <c r="I9" s="14">
+        <v>78</v>
+      </c>
+      <c r="J9" s="14">
+        <v>76</v>
+      </c>
+      <c r="K9" s="14">
+        <v>83</v>
+      </c>
+      <c r="L9" s="14">
+        <f t="shared" si="0"/>
+        <v>756</v>
+      </c>
+      <c r="M9" s="14">
+        <f t="shared" si="1"/>
+        <v>75.599999999999994</v>
+      </c>
+      <c r="N9" s="8">
+        <f>RANK(L9,L6:L35)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="14">
+        <v>91</v>
+      </c>
+      <c r="C10" s="14">
+        <v>85</v>
+      </c>
+      <c r="D10" s="14">
+        <v>79</v>
+      </c>
+      <c r="E10" s="14">
+        <v>92</v>
+      </c>
+      <c r="F10" s="14">
+        <v>86</v>
+      </c>
+      <c r="G10" s="14">
+        <v>81</v>
+      </c>
+      <c r="H10" s="14">
+        <v>83</v>
+      </c>
+      <c r="I10" s="14">
+        <v>90</v>
+      </c>
+      <c r="J10" s="14">
+        <v>82</v>
+      </c>
+      <c r="K10" s="14">
+        <v>82</v>
+      </c>
+      <c r="L10" s="14">
+        <f t="shared" si="0"/>
+        <v>851</v>
+      </c>
+      <c r="M10" s="14">
+        <f t="shared" si="1"/>
+        <v>85.1</v>
+      </c>
+      <c r="N10" s="8">
+        <f>RANK(L10,L6:L35)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="14">
+        <v>90</v>
+      </c>
+      <c r="C11" s="14">
+        <v>81</v>
+      </c>
+      <c r="D11" s="14">
+        <v>90</v>
+      </c>
+      <c r="E11" s="14">
+        <v>83</v>
+      </c>
+      <c r="F11" s="14">
+        <v>82</v>
+      </c>
+      <c r="G11" s="14">
+        <v>92</v>
+      </c>
+      <c r="H11" s="14">
+        <v>95</v>
+      </c>
+      <c r="I11" s="14">
+        <v>89</v>
+      </c>
+      <c r="J11" s="14">
+        <v>87</v>
+      </c>
+      <c r="K11" s="14">
+        <v>88</v>
+      </c>
+      <c r="L11" s="14">
+        <f t="shared" si="0"/>
+        <v>877</v>
+      </c>
+      <c r="M11" s="14">
+        <f t="shared" si="1"/>
+        <v>87.7</v>
+      </c>
+      <c r="N11" s="8">
+        <f>RANK(L11,L6:L35)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="14">
+        <v>82</v>
+      </c>
+      <c r="C12" s="14">
+        <v>89</v>
+      </c>
+      <c r="D12" s="14">
+        <v>94</v>
+      </c>
+      <c r="E12" s="14">
+        <v>91</v>
+      </c>
+      <c r="F12" s="14">
+        <v>86</v>
+      </c>
+      <c r="G12" s="14">
+        <v>87</v>
+      </c>
+      <c r="H12" s="14">
+        <v>80</v>
+      </c>
+      <c r="I12" s="14">
+        <v>83</v>
+      </c>
+      <c r="J12" s="14">
+        <v>86</v>
+      </c>
+      <c r="K12" s="14">
+        <v>80</v>
+      </c>
+      <c r="L12" s="14">
+        <f t="shared" si="0"/>
+        <v>858</v>
+      </c>
+      <c r="M12" s="14">
+        <f t="shared" si="1"/>
+        <v>85.8</v>
+      </c>
+      <c r="N12" s="8">
+        <f>RANK(L12,L6:L35)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="14">
+        <v>77</v>
+      </c>
+      <c r="C13" s="14">
+        <v>78</v>
+      </c>
+      <c r="D13" s="14">
+        <v>60</v>
+      </c>
+      <c r="E13" s="14">
+        <v>79</v>
+      </c>
+      <c r="F13" s="14">
+        <v>65</v>
+      </c>
+      <c r="G13" s="14">
+        <v>77</v>
+      </c>
+      <c r="H13" s="14">
+        <v>80</v>
+      </c>
+      <c r="I13" s="14">
+        <v>73</v>
+      </c>
+      <c r="J13" s="14">
+        <v>70</v>
+      </c>
+      <c r="K13" s="14">
+        <v>81</v>
+      </c>
+      <c r="L13" s="14">
+        <f t="shared" si="0"/>
+        <v>740</v>
+      </c>
+      <c r="M13" s="14">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="N13" s="8">
+        <f>RANK(L13,L6:L35)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A14" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="14">
+        <v>71</v>
+      </c>
+      <c r="C14" s="14">
+        <v>82</v>
+      </c>
+      <c r="D14" s="14">
+        <v>69</v>
+      </c>
+      <c r="E14" s="14">
+        <v>75</v>
+      </c>
+      <c r="F14" s="14">
+        <v>69</v>
+      </c>
+      <c r="G14" s="14">
+        <v>81</v>
+      </c>
+      <c r="H14" s="14">
+        <v>70</v>
+      </c>
+      <c r="I14" s="14">
+        <v>72</v>
+      </c>
+      <c r="J14" s="14">
+        <v>74</v>
+      </c>
+      <c r="K14" s="14">
+        <v>84</v>
+      </c>
+      <c r="L14" s="14">
+        <f t="shared" si="0"/>
+        <v>747</v>
+      </c>
+      <c r="M14" s="14">
+        <f t="shared" si="1"/>
+        <v>74.7</v>
+      </c>
+      <c r="N14" s="8">
+        <f>RANK(L14,L6:L35)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A15" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="14">
+        <v>85</v>
+      </c>
+      <c r="C15" s="14">
+        <v>81</v>
+      </c>
+      <c r="D15" s="14">
+        <v>84</v>
+      </c>
+      <c r="E15" s="14">
+        <v>88</v>
+      </c>
+      <c r="F15" s="14">
+        <v>83</v>
+      </c>
+      <c r="G15" s="14">
+        <v>81</v>
+      </c>
+      <c r="H15" s="14">
+        <v>89</v>
+      </c>
+      <c r="I15" s="14">
+        <v>88</v>
+      </c>
+      <c r="J15" s="14">
+        <v>82</v>
+      </c>
+      <c r="K15" s="14">
+        <v>85</v>
+      </c>
+      <c r="L15" s="14">
+        <f t="shared" si="0"/>
+        <v>846</v>
+      </c>
+      <c r="M15" s="14">
+        <f t="shared" si="1"/>
+        <v>84.6</v>
+      </c>
+      <c r="N15" s="8">
+        <f>RANK(L15,L6:L35)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A16" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="14">
+        <v>85</v>
+      </c>
+      <c r="C16" s="14">
+        <v>75</v>
+      </c>
+      <c r="D16" s="14">
+        <v>79</v>
+      </c>
+      <c r="E16" s="14">
+        <v>78</v>
+      </c>
+      <c r="F16" s="14">
+        <v>82</v>
+      </c>
+      <c r="G16" s="14">
+        <v>86</v>
+      </c>
+      <c r="H16" s="14">
+        <v>81</v>
+      </c>
+      <c r="I16" s="14">
+        <v>70</v>
+      </c>
+      <c r="J16" s="14">
+        <v>79</v>
+      </c>
+      <c r="K16" s="14">
+        <v>86</v>
+      </c>
+      <c r="L16" s="14">
+        <f t="shared" si="0"/>
+        <v>801</v>
+      </c>
+      <c r="M16" s="14">
+        <f t="shared" si="1"/>
+        <v>80.099999999999994</v>
+      </c>
+      <c r="N16" s="8">
+        <f>RANK(L16,L6:L35)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="14">
+        <v>91</v>
+      </c>
+      <c r="C17" s="14">
+        <v>92</v>
+      </c>
+      <c r="D17" s="14">
+        <v>90</v>
+      </c>
+      <c r="E17" s="14">
+        <v>100</v>
+      </c>
+      <c r="F17" s="14">
+        <v>91</v>
+      </c>
+      <c r="G17" s="14">
+        <v>91</v>
+      </c>
+      <c r="H17" s="14">
+        <v>92</v>
+      </c>
+      <c r="I17" s="14">
+        <v>92</v>
+      </c>
+      <c r="J17" s="14">
+        <v>92</v>
+      </c>
+      <c r="K17" s="14">
+        <v>91</v>
+      </c>
+      <c r="L17" s="14">
+        <f t="shared" si="0"/>
+        <v>922</v>
+      </c>
+      <c r="M17" s="14">
+        <f t="shared" si="1"/>
+        <v>92.2</v>
+      </c>
+      <c r="N17" s="8">
+        <f>RANK(L17,L6:L35)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A18" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="14">
+        <v>94</v>
+      </c>
+      <c r="C18" s="14">
+        <v>81</v>
+      </c>
+      <c r="D18" s="14">
+        <v>93</v>
+      </c>
+      <c r="E18" s="14">
+        <v>69</v>
+      </c>
+      <c r="F18" s="14">
+        <v>82</v>
+      </c>
+      <c r="G18" s="14">
+        <v>90</v>
+      </c>
+      <c r="H18" s="14">
+        <v>91</v>
+      </c>
+      <c r="I18" s="14">
+        <v>92</v>
+      </c>
+      <c r="J18" s="14">
+        <v>89</v>
+      </c>
+      <c r="K18" s="14">
+        <v>81</v>
+      </c>
+      <c r="L18" s="14">
+        <f t="shared" si="0"/>
+        <v>862</v>
+      </c>
+      <c r="M18" s="14">
+        <f t="shared" si="1"/>
+        <v>86.2</v>
+      </c>
+      <c r="N18" s="8">
+        <f>RANK(L18,L6:L35)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A19" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="14">
+        <v>87</v>
+      </c>
+      <c r="C19" s="14">
+        <v>89</v>
+      </c>
+      <c r="D19" s="14">
+        <v>87</v>
+      </c>
+      <c r="E19" s="14">
+        <v>86</v>
+      </c>
+      <c r="F19" s="14">
+        <v>82</v>
+      </c>
+      <c r="G19" s="14">
+        <v>80</v>
+      </c>
+      <c r="H19" s="14">
+        <v>84</v>
+      </c>
+      <c r="I19" s="14">
+        <v>92</v>
+      </c>
+      <c r="J19" s="14">
+        <v>90</v>
+      </c>
+      <c r="K19" s="14">
+        <v>89</v>
+      </c>
+      <c r="L19" s="14">
+        <f t="shared" si="0"/>
+        <v>866</v>
+      </c>
+      <c r="M19" s="14">
+        <f t="shared" si="1"/>
+        <v>86.6</v>
+      </c>
+      <c r="N19" s="8">
+        <f>RANK(L19,L6:L35)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A20" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" s="14">
+        <v>78</v>
+      </c>
+      <c r="C20" s="14">
+        <v>75</v>
+      </c>
+      <c r="D20" s="14">
+        <v>71</v>
+      </c>
+      <c r="E20" s="14">
+        <v>75</v>
+      </c>
+      <c r="F20" s="14">
+        <v>79</v>
+      </c>
+      <c r="G20" s="14">
+        <v>70</v>
+      </c>
+      <c r="H20" s="14">
+        <v>72</v>
+      </c>
+      <c r="I20" s="14">
+        <v>73</v>
+      </c>
+      <c r="J20" s="14">
+        <v>76</v>
+      </c>
+      <c r="K20" s="14">
+        <v>77</v>
+      </c>
+      <c r="L20" s="14">
+        <f t="shared" si="0"/>
+        <v>746</v>
+      </c>
+      <c r="M20" s="14">
+        <f t="shared" si="1"/>
+        <v>74.599999999999994</v>
+      </c>
+      <c r="N20" s="8">
+        <f>RANK(L20,L6:L35)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A21" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="14">
+        <v>93</v>
+      </c>
+      <c r="C21" s="14">
+        <v>91</v>
+      </c>
+      <c r="D21" s="14">
+        <v>90</v>
+      </c>
+      <c r="E21" s="14">
+        <v>89</v>
+      </c>
+      <c r="F21" s="14">
+        <v>82</v>
+      </c>
+      <c r="G21" s="14">
+        <v>85</v>
+      </c>
+      <c r="H21" s="14">
+        <v>87</v>
+      </c>
+      <c r="I21" s="14">
+        <v>88</v>
+      </c>
+      <c r="J21" s="14">
+        <v>87</v>
+      </c>
+      <c r="K21" s="14">
+        <v>84</v>
+      </c>
+      <c r="L21" s="14">
+        <f t="shared" si="0"/>
+        <v>876</v>
+      </c>
+      <c r="M21" s="14">
+        <f t="shared" si="1"/>
+        <v>87.6</v>
+      </c>
+      <c r="N21" s="8">
+        <f>RANK(L21,L6:L35)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A22" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="14">
+        <v>88</v>
+      </c>
+      <c r="C22" s="14">
+        <v>82</v>
+      </c>
+      <c r="D22" s="14">
+        <v>80</v>
+      </c>
+      <c r="E22" s="14">
+        <v>81</v>
+      </c>
+      <c r="F22" s="14">
+        <v>84</v>
+      </c>
+      <c r="G22" s="14">
+        <v>81</v>
+      </c>
+      <c r="H22" s="14">
+        <v>80</v>
+      </c>
+      <c r="I22" s="14">
+        <v>82</v>
+      </c>
+      <c r="J22" s="14">
+        <v>91</v>
+      </c>
+      <c r="K22" s="14">
+        <v>87</v>
+      </c>
+      <c r="L22" s="14">
+        <f t="shared" si="0"/>
+        <v>836</v>
+      </c>
+      <c r="M22" s="14">
+        <f t="shared" si="1"/>
+        <v>83.6</v>
+      </c>
+      <c r="N22" s="8">
+        <f>RANK(L22,L6:L35)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A23" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="14">
+        <v>93</v>
+      </c>
+      <c r="C23" s="14">
+        <v>94</v>
+      </c>
+      <c r="D23" s="14">
+        <v>95</v>
+      </c>
+      <c r="E23" s="14">
+        <v>92</v>
+      </c>
+      <c r="F23" s="14">
+        <v>90</v>
+      </c>
+      <c r="G23" s="14">
+        <v>90</v>
+      </c>
+      <c r="H23" s="14">
+        <v>98</v>
+      </c>
+      <c r="I23" s="14">
+        <v>100</v>
+      </c>
+      <c r="J23" s="14">
+        <v>99</v>
+      </c>
+      <c r="K23" s="14">
+        <v>94</v>
+      </c>
+      <c r="L23" s="14">
+        <f t="shared" si="0"/>
+        <v>945</v>
+      </c>
+      <c r="M23" s="14">
+        <f t="shared" si="1"/>
+        <v>94.5</v>
+      </c>
+      <c r="N23" s="8">
+        <f>RANK(L23,L6:L35)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A24" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="14">
+        <v>84</v>
+      </c>
+      <c r="C24" s="14">
+        <v>90</v>
+      </c>
+      <c r="D24" s="14">
+        <v>91</v>
+      </c>
+      <c r="E24" s="14">
+        <v>93</v>
+      </c>
+      <c r="F24" s="14">
+        <v>90</v>
+      </c>
+      <c r="G24" s="14">
+        <v>92</v>
+      </c>
+      <c r="H24" s="14">
+        <v>91</v>
+      </c>
+      <c r="I24" s="14">
+        <v>81</v>
+      </c>
+      <c r="J24" s="14">
+        <v>85</v>
+      </c>
+      <c r="K24" s="14">
+        <v>84</v>
+      </c>
+      <c r="L24" s="14">
+        <f t="shared" si="0"/>
+        <v>881</v>
+      </c>
+      <c r="M24" s="14">
+        <f t="shared" si="1"/>
+        <v>88.1</v>
+      </c>
+      <c r="N24" s="8">
+        <f>RANK(L24,L6:L35)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A25" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="14">
+        <v>83</v>
+      </c>
+      <c r="C25" s="14">
+        <v>75</v>
+      </c>
+      <c r="D25" s="14">
+        <v>74</v>
+      </c>
+      <c r="E25" s="14">
+        <v>76</v>
+      </c>
+      <c r="F25" s="14">
+        <v>78</v>
+      </c>
+      <c r="G25" s="14">
+        <v>89</v>
+      </c>
+      <c r="H25" s="14">
+        <v>90</v>
+      </c>
+      <c r="I25" s="14">
+        <v>87</v>
+      </c>
+      <c r="J25" s="14">
+        <v>82</v>
+      </c>
+      <c r="K25" s="14">
+        <v>88</v>
+      </c>
+      <c r="L25" s="14">
+        <f t="shared" si="0"/>
+        <v>822</v>
+      </c>
+      <c r="M25" s="14">
+        <f t="shared" si="1"/>
+        <v>82.2</v>
+      </c>
+      <c r="N25" s="8">
+        <f>RANK(L25,L6:L35)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A26" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" s="14">
+        <v>89</v>
+      </c>
+      <c r="C26" s="14">
+        <v>87</v>
+      </c>
+      <c r="D26" s="14">
+        <v>83</v>
+      </c>
+      <c r="E26" s="14">
+        <v>80</v>
+      </c>
+      <c r="F26" s="14">
+        <v>91</v>
+      </c>
+      <c r="G26" s="14">
+        <v>72</v>
+      </c>
+      <c r="H26" s="14">
+        <v>92</v>
+      </c>
+      <c r="I26" s="14">
+        <v>85</v>
+      </c>
+      <c r="J26" s="14">
+        <v>89</v>
+      </c>
+      <c r="K26" s="14">
+        <v>94</v>
+      </c>
+      <c r="L26" s="14">
+        <f t="shared" si="0"/>
+        <v>862</v>
+      </c>
+      <c r="M26" s="14">
+        <f t="shared" si="1"/>
+        <v>86.2</v>
+      </c>
+      <c r="N26" s="8">
+        <f>RANK(L26,L6:L35)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A27" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" s="14">
+        <v>89</v>
+      </c>
+      <c r="C27" s="14">
+        <v>87</v>
+      </c>
+      <c r="D27" s="14">
+        <v>91</v>
+      </c>
+      <c r="E27" s="14">
+        <v>90</v>
+      </c>
+      <c r="F27" s="14">
+        <v>90</v>
+      </c>
+      <c r="G27" s="14">
+        <v>83</v>
+      </c>
+      <c r="H27" s="14">
+        <v>87</v>
+      </c>
+      <c r="I27" s="14">
+        <v>91</v>
+      </c>
+      <c r="J27" s="14">
+        <v>90</v>
+      </c>
+      <c r="K27" s="14">
+        <v>94</v>
+      </c>
+      <c r="L27" s="14">
+        <f t="shared" si="0"/>
+        <v>892</v>
+      </c>
+      <c r="M27" s="14">
+        <f t="shared" si="1"/>
+        <v>89.2</v>
+      </c>
+      <c r="N27" s="8">
+        <f>RANK(L27,L6:L35)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A28" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" s="14">
+        <v>87</v>
+      </c>
+      <c r="C28" s="14">
+        <v>91</v>
+      </c>
+      <c r="D28" s="14">
+        <v>90</v>
+      </c>
+      <c r="E28" s="14">
+        <v>90</v>
+      </c>
+      <c r="F28" s="14">
+        <v>81</v>
+      </c>
+      <c r="G28" s="14">
+        <v>79</v>
+      </c>
+      <c r="H28" s="14">
+        <v>78</v>
+      </c>
+      <c r="I28" s="14">
+        <v>79</v>
+      </c>
+      <c r="J28" s="14">
+        <v>80</v>
+      </c>
+      <c r="K28" s="14">
+        <v>87</v>
+      </c>
+      <c r="L28" s="14">
+        <f t="shared" si="0"/>
+        <v>842</v>
+      </c>
+      <c r="M28" s="14">
+        <f t="shared" si="1"/>
+        <v>84.2</v>
+      </c>
+      <c r="N28" s="8">
+        <f>RANK(L28,L6:L35)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A29" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" s="14">
+        <v>79</v>
+      </c>
+      <c r="C29" s="14">
+        <v>86</v>
+      </c>
+      <c r="D29" s="14">
+        <v>75</v>
+      </c>
+      <c r="E29" s="14">
+        <v>75</v>
+      </c>
+      <c r="F29" s="14">
+        <v>71</v>
+      </c>
+      <c r="G29" s="14">
+        <v>82</v>
+      </c>
+      <c r="H29" s="14">
+        <v>85</v>
+      </c>
+      <c r="I29" s="14">
+        <v>80</v>
+      </c>
+      <c r="J29" s="14">
+        <v>93</v>
+      </c>
+      <c r="K29" s="14">
+        <v>94</v>
+      </c>
+      <c r="L29" s="14">
+        <f t="shared" si="0"/>
+        <v>820</v>
+      </c>
+      <c r="M29" s="14">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="N29" s="8">
+        <f>RANK(L29,L6:L35)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A30" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="14">
+        <v>80</v>
+      </c>
+      <c r="C30" s="14">
+        <v>79</v>
+      </c>
+      <c r="D30" s="14">
+        <v>87</v>
+      </c>
+      <c r="E30" s="14">
+        <v>89</v>
+      </c>
+      <c r="F30" s="14">
+        <v>91</v>
+      </c>
+      <c r="G30" s="14">
+        <v>90</v>
+      </c>
+      <c r="H30" s="14">
+        <v>94</v>
+      </c>
+      <c r="I30" s="14">
+        <v>93</v>
+      </c>
+      <c r="J30" s="14">
+        <v>91</v>
+      </c>
+      <c r="K30" s="14">
+        <v>94</v>
+      </c>
+      <c r="L30" s="14">
+        <f t="shared" si="0"/>
+        <v>888</v>
+      </c>
+      <c r="M30" s="14">
+        <f t="shared" si="1"/>
+        <v>88.8</v>
+      </c>
+      <c r="N30" s="8">
+        <f>RANK(L30,L6:L35)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A31" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="14">
+        <v>69</v>
+      </c>
+      <c r="C31" s="14">
+        <v>67</v>
+      </c>
+      <c r="D31" s="14">
+        <v>71</v>
+      </c>
+      <c r="E31" s="14">
+        <v>69</v>
+      </c>
+      <c r="F31" s="14">
+        <v>71</v>
+      </c>
+      <c r="G31" s="14">
+        <v>69</v>
+      </c>
+      <c r="H31" s="14">
+        <v>69</v>
+      </c>
+      <c r="I31" s="14">
+        <v>60</v>
+      </c>
+      <c r="J31" s="14">
+        <v>71</v>
+      </c>
+      <c r="K31" s="14">
+        <v>73</v>
+      </c>
+      <c r="L31" s="14">
+        <f t="shared" si="0"/>
+        <v>689</v>
+      </c>
+      <c r="M31" s="14">
+        <f t="shared" si="1"/>
+        <v>68.900000000000006</v>
+      </c>
+      <c r="N31" s="8">
+        <f>RANK(L31,L6:L35)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A32" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" s="14">
+        <v>73</v>
+      </c>
+      <c r="C32" s="14">
+        <v>77</v>
+      </c>
+      <c r="D32" s="14">
+        <v>78</v>
+      </c>
+      <c r="E32" s="14">
+        <v>82</v>
+      </c>
+      <c r="F32" s="14">
+        <v>84</v>
+      </c>
+      <c r="G32" s="14">
+        <v>90</v>
+      </c>
+      <c r="H32" s="14">
+        <v>91</v>
+      </c>
+      <c r="I32" s="14">
+        <v>75</v>
+      </c>
+      <c r="J32" s="14">
+        <v>80</v>
+      </c>
+      <c r="K32" s="14">
+        <v>85</v>
+      </c>
+      <c r="L32" s="14">
+        <f t="shared" si="0"/>
+        <v>815</v>
+      </c>
+      <c r="M32" s="14">
+        <f t="shared" si="1"/>
+        <v>81.5</v>
+      </c>
+      <c r="N32" s="8">
+        <f>RANK(L32,L6:L35)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A33" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" s="14">
+        <v>93</v>
+      </c>
+      <c r="C33" s="14">
+        <v>87</v>
+      </c>
+      <c r="D33" s="14">
+        <v>85</v>
+      </c>
+      <c r="E33" s="14">
+        <v>83</v>
+      </c>
+      <c r="F33" s="14">
+        <v>71</v>
+      </c>
+      <c r="G33" s="14">
+        <v>80</v>
+      </c>
+      <c r="H33" s="14">
+        <v>82</v>
+      </c>
+      <c r="I33" s="14">
+        <v>85</v>
+      </c>
+      <c r="J33" s="14">
+        <v>81</v>
+      </c>
+      <c r="K33" s="14">
+        <v>84</v>
+      </c>
+      <c r="L33" s="14">
+        <f t="shared" si="0"/>
+        <v>831</v>
+      </c>
+      <c r="M33" s="14">
+        <f t="shared" si="1"/>
+        <v>83.1</v>
+      </c>
+      <c r="N33" s="8">
+        <f>RANK(L33,L6:L35)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A34" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B34" s="14">
+        <v>85</v>
+      </c>
+      <c r="C34" s="14">
+        <v>90</v>
+      </c>
+      <c r="D34" s="14">
+        <v>93</v>
+      </c>
+      <c r="E34" s="14">
+        <v>91</v>
+      </c>
+      <c r="F34" s="14">
+        <v>91</v>
+      </c>
+      <c r="G34" s="14">
+        <v>92</v>
+      </c>
+      <c r="H34" s="14">
+        <v>87</v>
+      </c>
+      <c r="I34" s="14">
+        <v>85</v>
+      </c>
+      <c r="J34" s="14">
+        <v>85</v>
+      </c>
+      <c r="K34" s="14">
+        <v>80</v>
+      </c>
+      <c r="L34" s="14">
+        <f t="shared" si="0"/>
+        <v>879</v>
+      </c>
+      <c r="M34" s="14">
+        <f t="shared" si="1"/>
+        <v>87.9</v>
+      </c>
+      <c r="N34" s="8">
+        <f>RANK(L34,L6:L35)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A35" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B35" s="14">
+        <v>89</v>
+      </c>
+      <c r="C35" s="14">
+        <v>87</v>
+      </c>
+      <c r="D35" s="14">
+        <v>83</v>
+      </c>
+      <c r="E35" s="14">
+        <v>86</v>
+      </c>
+      <c r="F35" s="14">
+        <v>81</v>
+      </c>
+      <c r="G35" s="14">
+        <v>80</v>
+      </c>
+      <c r="H35" s="14">
+        <v>92</v>
+      </c>
+      <c r="I35" s="14">
+        <v>80</v>
+      </c>
+      <c r="J35" s="14">
+        <v>94</v>
+      </c>
+      <c r="K35" s="14">
+        <v>92</v>
+      </c>
+      <c r="L35" s="14">
+        <f t="shared" si="0"/>
+        <v>864</v>
+      </c>
+      <c r="M35" s="14">
+        <f t="shared" si="1"/>
+        <v>86.4</v>
+      </c>
+      <c r="N35" s="8">
+        <f>RANK(L35,L6:L35)</f>
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="M1:M3"/>
+    <mergeCell ref="N1:N3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>